<commit_message>
Création des images sur ggplot
</commit_message>
<xml_diff>
--- a/picross_5X5.xlsx
+++ b/picross_5X5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\OneDrive\Bureau\Cours fac\S2\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\OneDrive\Documents\projet_r\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897F8F72-8E85-4CDC-95D0-636D2AE00F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB805B4-54BC-4735-BE1C-AEB05237DAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FFEDFBDE-2F30-47DF-A7CD-97FB90A4FBBE}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>